<commit_message>
Data Act 15-09 4pm
</commit_message>
<xml_diff>
--- a/Data/Dataset_Unificado.xlsx
+++ b/Data/Dataset_Unificado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f15395a9ed9a48f/Imágenes/Proyectos/Indicadores/Prospectiva/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f15395a9ed9a48f/Imágenes/Proyectos/Indicadores/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_C54DB9D477E07092D1C9E253F65DD242EE9209D1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1354F346-0DCC-4AB9-9773-CE7C4375EC46}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_C54DB9D477E07092D1C9E253F65DD242EE9209D1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BDE396F-EEBE-478A-A2BD-15606BB7F8E9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1828,12 +1828,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AC427"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I321" workbookViewId="0">
-      <selection activeCell="W425" sqref="W425"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1929,7 +1926,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>14</v>
       </c>
@@ -2018,7 +2015,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>14</v>
       </c>
@@ -2107,7 +2104,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>14</v>
       </c>
@@ -2196,7 +2193,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>14</v>
       </c>
@@ -2285,7 +2282,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>14</v>
       </c>
@@ -2374,7 +2371,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>14</v>
       </c>
@@ -2819,7 +2816,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>96</v>
       </c>
@@ -2908,7 +2905,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>96</v>
       </c>
@@ -2997,7 +2994,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>96</v>
       </c>
@@ -3086,7 +3083,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>96</v>
       </c>
@@ -3175,7 +3172,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>97</v>
       </c>
@@ -3264,7 +3261,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>97</v>
       </c>
@@ -3347,7 +3344,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>97</v>
       </c>
@@ -3424,7 +3421,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>97</v>
       </c>
@@ -3501,7 +3498,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>98</v>
       </c>
@@ -3584,7 +3581,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>98</v>
       </c>
@@ -3673,7 +3670,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>98</v>
       </c>
@@ -3756,7 +3753,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>98</v>
       </c>
@@ -3981,7 +3978,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>148</v>
       </c>
@@ -4070,7 +4067,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>148</v>
       </c>
@@ -4159,7 +4156,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>148</v>
       </c>
@@ -4248,7 +4245,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>148</v>
       </c>
@@ -4331,7 +4328,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>193</v>
       </c>
@@ -4420,7 +4417,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>193</v>
       </c>
@@ -4509,7 +4506,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>193</v>
       </c>
@@ -4598,7 +4595,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>193</v>
       </c>
@@ -4687,7 +4684,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>193</v>
       </c>
@@ -4776,7 +4773,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>193</v>
       </c>
@@ -4859,7 +4856,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>194</v>
       </c>
@@ -4948,7 +4945,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>194</v>
       </c>
@@ -5037,7 +5034,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>194</v>
       </c>
@@ -5126,7 +5123,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>194</v>
       </c>
@@ -5215,7 +5212,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>194</v>
       </c>
@@ -5627,7 +5624,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>203</v>
       </c>
@@ -5716,7 +5713,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>203</v>
       </c>
@@ -5805,7 +5802,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>203</v>
       </c>
@@ -5894,7 +5891,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>203</v>
       </c>
@@ -5983,7 +5980,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>203</v>
       </c>
@@ -6072,7 +6069,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>203</v>
       </c>
@@ -6161,7 +6158,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>204</v>
       </c>
@@ -6250,7 +6247,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>204</v>
       </c>
@@ -6339,7 +6336,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>204</v>
       </c>
@@ -6428,7 +6425,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>204</v>
       </c>
@@ -6517,7 +6514,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>204</v>
       </c>
@@ -6606,7 +6603,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>204</v>
       </c>
@@ -6695,7 +6692,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>205</v>
       </c>
@@ -6784,7 +6781,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>205</v>
       </c>
@@ -6873,7 +6870,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>205</v>
       </c>
@@ -6962,7 +6959,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>205</v>
       </c>
@@ -7051,7 +7048,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>206</v>
       </c>
@@ -7140,7 +7137,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>206</v>
       </c>
@@ -7229,7 +7226,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>206</v>
       </c>
@@ -7306,7 +7303,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>207</v>
       </c>
@@ -7395,7 +7392,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>207</v>
       </c>
@@ -7484,7 +7481,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>207</v>
       </c>
@@ -7573,7 +7570,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>207</v>
       </c>
@@ -7662,7 +7659,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>228</v>
       </c>
@@ -7745,7 +7742,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>228</v>
       </c>
@@ -7816,7 +7813,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>244</v>
       </c>
@@ -7899,7 +7896,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>244</v>
       </c>
@@ -7982,7 +7979,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>245</v>
       </c>
@@ -8071,7 +8068,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>245</v>
       </c>
@@ -8160,7 +8157,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>245</v>
       </c>
@@ -8249,7 +8246,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="75" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>245</v>
       </c>
@@ -8338,7 +8335,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>245</v>
       </c>
@@ -8427,7 +8424,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>245</v>
       </c>
@@ -8510,7 +8507,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="78" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>274</v>
       </c>
@@ -8599,7 +8596,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>274</v>
       </c>
@@ -8688,7 +8685,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="80" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>274</v>
       </c>
@@ -8777,7 +8774,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>274</v>
       </c>
@@ -8866,7 +8863,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="82" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>274</v>
       </c>
@@ -8955,7 +8952,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="83" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>274</v>
       </c>
@@ -9044,7 +9041,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="84" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>276</v>
       </c>
@@ -9127,7 +9124,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>276</v>
       </c>
@@ -9210,7 +9207,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>276</v>
       </c>
@@ -9293,7 +9290,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="87" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>276</v>
       </c>
@@ -9376,7 +9373,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>276</v>
       </c>
@@ -9459,7 +9456,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>276</v>
       </c>
@@ -9542,7 +9539,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="90" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>277</v>
       </c>
@@ -9622,7 +9619,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>277</v>
       </c>
@@ -9702,7 +9699,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>277</v>
       </c>
@@ -9782,7 +9779,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>277</v>
       </c>
@@ -9862,7 +9859,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="94" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>323</v>
       </c>
@@ -9945,7 +9942,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="95" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>323</v>
       </c>
@@ -10028,7 +10025,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="96" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>323</v>
       </c>
@@ -10111,7 +10108,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="97" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>323</v>
       </c>
@@ -10194,7 +10191,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="98" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>323</v>
       </c>
@@ -10271,7 +10268,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>325</v>
       </c>
@@ -10360,7 +10357,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="100" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>325</v>
       </c>
@@ -10449,7 +10446,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>325</v>
       </c>
@@ -10538,7 +10535,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="102" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>325</v>
       </c>
@@ -10615,7 +10612,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="103" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>325</v>
       </c>
@@ -10704,7 +10701,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="104" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>325</v>
       </c>
@@ -10793,7 +10790,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="105" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>331</v>
       </c>
@@ -10876,7 +10873,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="106" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>331</v>
       </c>
@@ -11795,7 +11792,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="117" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>339</v>
       </c>
@@ -11884,7 +11881,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="118" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>339</v>
       </c>
@@ -12139,7 +12136,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="121" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>361</v>
       </c>
@@ -12222,7 +12219,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="122" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>361</v>
       </c>
@@ -12299,7 +12296,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="123" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>364</v>
       </c>
@@ -12388,7 +12385,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="124" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>364</v>
       </c>
@@ -12477,7 +12474,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="125" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>364</v>
       </c>
@@ -12566,7 +12563,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="126" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>364</v>
       </c>
@@ -12655,7 +12652,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="127" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>367</v>
       </c>
@@ -12744,7 +12741,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="128" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>367</v>
       </c>
@@ -12833,7 +12830,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="129" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>369</v>
       </c>
@@ -12916,7 +12913,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="130" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>369</v>
       </c>
@@ -12999,7 +12996,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="131" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>369</v>
       </c>
@@ -13088,7 +13085,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="132" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>369</v>
       </c>
@@ -13177,7 +13174,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="133" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>376</v>
       </c>
@@ -13266,7 +13263,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="134" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>376</v>
       </c>
@@ -13355,7 +13352,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="135" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>376</v>
       </c>
@@ -13444,7 +13441,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="136" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>376</v>
       </c>
@@ -13533,7 +13530,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="137" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>376</v>
       </c>
@@ -13622,7 +13619,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="138" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>376</v>
       </c>
@@ -13711,7 +13708,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="139" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>377</v>
       </c>
@@ -13800,7 +13797,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="140" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>377</v>
       </c>
@@ -13889,7 +13886,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="141" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>377</v>
       </c>
@@ -13978,7 +13975,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="142" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>377</v>
       </c>
@@ -14067,7 +14064,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="143" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>379</v>
       </c>
@@ -14156,7 +14153,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="144" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>379</v>
       </c>
@@ -14245,7 +14242,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="145" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>379</v>
       </c>
@@ -14334,7 +14331,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="146" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>379</v>
       </c>
@@ -14423,7 +14420,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="147" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>379</v>
       </c>
@@ -14512,7 +14509,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="148" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>379</v>
       </c>
@@ -15135,7 +15132,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="155" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>423</v>
       </c>
@@ -15218,7 +15215,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="156" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>423</v>
       </c>
@@ -15301,7 +15298,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="157" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>423</v>
       </c>
@@ -15384,7 +15381,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="158" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>424</v>
       </c>
@@ -15467,7 +15464,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="159" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>424</v>
       </c>
@@ -15550,7 +15547,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="160" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>424</v>
       </c>
@@ -15633,7 +15630,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="161" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>460</v>
       </c>
@@ -16048,7 +16045,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="166" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>466</v>
       </c>
@@ -16131,7 +16128,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="167" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>466</v>
       </c>
@@ -16374,7 +16371,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="170" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>476</v>
       </c>
@@ -16457,7 +16454,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="171" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>476</v>
       </c>
@@ -16540,7 +16537,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="172" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>14.1</v>
       </c>
@@ -16629,7 +16626,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="173" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>14.1</v>
       </c>
@@ -16718,7 +16715,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="174" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>14.1</v>
       </c>
@@ -16807,7 +16804,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="175" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>14.1</v>
       </c>
@@ -16896,7 +16893,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="176" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>14.1</v>
       </c>
@@ -16985,7 +16982,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="177" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>14.2</v>
       </c>
@@ -17074,7 +17071,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="178" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>14.2</v>
       </c>
@@ -17163,7 +17160,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="179" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>14.2</v>
       </c>
@@ -17252,7 +17249,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="180" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>14.2</v>
       </c>
@@ -17341,7 +17338,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="181" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>14.2</v>
       </c>
@@ -17430,7 +17427,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="182" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>14.3</v>
       </c>
@@ -17519,7 +17516,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="183" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>14.3</v>
       </c>
@@ -17608,7 +17605,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="184" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>14.3</v>
       </c>
@@ -17697,7 +17694,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="185" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>14.3</v>
       </c>
@@ -17786,7 +17783,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="186" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>14.3</v>
       </c>
@@ -17875,7 +17872,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="187" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>14.4</v>
       </c>
@@ -17964,7 +17961,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="188" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>14.4</v>
       </c>
@@ -18053,7 +18050,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="189" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>14.4</v>
       </c>
@@ -18142,7 +18139,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="190" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>14.4</v>
       </c>
@@ -18231,7 +18228,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="191" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>14.4</v>
       </c>
@@ -19530,7 +19527,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="206" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>96</v>
       </c>
@@ -19619,7 +19616,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="207" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>97</v>
       </c>
@@ -19696,7 +19693,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="208" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>97</v>
       </c>
@@ -19773,7 +19770,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="209" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>98</v>
       </c>
@@ -19850,7 +19847,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="210" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>98</v>
       </c>
@@ -19939,7 +19936,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="211" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>14.1</v>
       </c>
@@ -20028,7 +20025,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="212" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>14.2</v>
       </c>
@@ -20117,7 +20114,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="213" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>14.3</v>
       </c>
@@ -20206,7 +20203,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="214" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>14.4</v>
       </c>
@@ -20295,7 +20292,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="215" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>194</v>
       </c>
@@ -20384,7 +20381,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="216" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>476</v>
       </c>
@@ -20473,7 +20470,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="217" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>148</v>
       </c>
@@ -20562,7 +20559,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="218" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>339</v>
       </c>
@@ -20651,7 +20648,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="219" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>325</v>
       </c>
@@ -20740,7 +20737,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="220" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>323</v>
       </c>
@@ -20829,7 +20826,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="221" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>276</v>
       </c>
@@ -20918,7 +20915,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="222" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>14</v>
       </c>
@@ -21007,7 +21004,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="223" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>379</v>
       </c>
@@ -21096,7 +21093,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="224" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>274</v>
       </c>
@@ -21185,7 +21182,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="225" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>14.1</v>
       </c>
@@ -21274,7 +21271,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="226" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>14.2</v>
       </c>
@@ -21363,7 +21360,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="227" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>14.3</v>
       </c>
@@ -21452,7 +21449,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="228" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>14.4</v>
       </c>
@@ -21541,7 +21538,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>98</v>
       </c>
@@ -21630,7 +21627,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="230" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>194</v>
       </c>
@@ -21719,7 +21716,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="231" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>193</v>
       </c>
@@ -21808,7 +21805,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>245</v>
       </c>
@@ -21897,7 +21894,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>205</v>
       </c>
@@ -21986,7 +21983,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="234" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>204</v>
       </c>
@@ -22075,7 +22072,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="235" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>364</v>
       </c>
@@ -22164,7 +22161,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="236" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>376</v>
       </c>
@@ -22253,7 +22250,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="237" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>203</v>
       </c>
@@ -22342,7 +22339,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="238" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>207</v>
       </c>
@@ -22431,7 +22428,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="239" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>369</v>
       </c>
@@ -22520,7 +22517,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="240" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>331</v>
       </c>
@@ -22867,7 +22864,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="244" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>277</v>
       </c>
@@ -23285,7 +23282,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="249" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>14</v>
       </c>
@@ -23371,7 +23368,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="250" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>14</v>
       </c>
@@ -23457,7 +23454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="251" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>14</v>
       </c>
@@ -23801,7 +23798,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="255" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>96</v>
       </c>
@@ -23887,7 +23884,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="256" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>96</v>
       </c>
@@ -23973,7 +23970,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="257" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>96</v>
       </c>
@@ -24059,7 +24056,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="258" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>97</v>
       </c>
@@ -24145,7 +24142,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="259" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>97</v>
       </c>
@@ -24225,7 +24222,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="260" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>97</v>
       </c>
@@ -24305,7 +24302,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="261" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>98</v>
       </c>
@@ -24391,7 +24388,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="262" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>98</v>
       </c>
@@ -24477,7 +24474,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="263" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>98</v>
       </c>
@@ -24646,7 +24643,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="265" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>148</v>
       </c>
@@ -24732,7 +24729,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="266" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>148</v>
       </c>
@@ -24818,7 +24815,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="267" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>148</v>
       </c>
@@ -24904,7 +24901,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="268" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>193</v>
       </c>
@@ -24990,7 +24987,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="269" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>193</v>
       </c>
@@ -25076,7 +25073,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="270" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>193</v>
       </c>
@@ -25162,7 +25159,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="271" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>194</v>
       </c>
@@ -25248,7 +25245,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="272" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>194</v>
       </c>
@@ -25334,7 +25331,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="273" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>194</v>
       </c>
@@ -25749,7 +25746,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="278" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>203</v>
       </c>
@@ -25835,7 +25832,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="279" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>203</v>
       </c>
@@ -25921,7 +25918,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="280" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>203</v>
       </c>
@@ -26007,7 +26004,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="281" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>204</v>
       </c>
@@ -26081,7 +26078,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="282" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>204</v>
       </c>
@@ -26167,7 +26164,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="283" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>204</v>
       </c>
@@ -26253,7 +26250,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="284" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>205</v>
       </c>
@@ -26339,7 +26336,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="285" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>205</v>
       </c>
@@ -26425,7 +26422,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="286" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>206</v>
       </c>
@@ -26511,7 +26508,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="287" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>206</v>
       </c>
@@ -26597,7 +26594,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="288" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>207</v>
       </c>
@@ -26683,7 +26680,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="289" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>207</v>
       </c>
@@ -26769,7 +26766,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="290" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>228</v>
       </c>
@@ -26855,7 +26852,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="291" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>228</v>
       </c>
@@ -26941,7 +26938,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="292" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>244</v>
       </c>
@@ -27027,7 +27024,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="293" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>244</v>
       </c>
@@ -27113,7 +27110,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="294" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>244</v>
       </c>
@@ -27199,7 +27196,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="295" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>245</v>
       </c>
@@ -27285,7 +27282,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="296" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>245</v>
       </c>
@@ -27371,7 +27368,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="297" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>245</v>
       </c>
@@ -27457,7 +27454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="298" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>476</v>
       </c>
@@ -27543,7 +27540,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="299" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>274</v>
       </c>
@@ -27629,7 +27626,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="300" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>274</v>
       </c>
@@ -27715,7 +27712,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="301" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>274</v>
       </c>
@@ -27801,7 +27798,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="302" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>276</v>
       </c>
@@ -27887,7 +27884,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="303" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>276</v>
       </c>
@@ -27973,7 +27970,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="304" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>276</v>
       </c>
@@ -28059,7 +28056,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="305" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>277</v>
       </c>
@@ -28142,7 +28139,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="306" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>277</v>
       </c>
@@ -28225,7 +28222,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="307" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>323</v>
       </c>
@@ -28311,7 +28308,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="308" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>323</v>
       </c>
@@ -28397,7 +28394,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="309" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>323</v>
       </c>
@@ -28483,7 +28480,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="310" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>325</v>
       </c>
@@ -28569,7 +28566,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="311" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>325</v>
       </c>
@@ -28655,7 +28652,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="312" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>325</v>
       </c>
@@ -28741,7 +28738,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="313" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>331</v>
       </c>
@@ -28818,7 +28815,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="314" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>331</v>
       </c>
@@ -29577,7 +29574,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="323" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>339</v>
       </c>
@@ -29663,7 +29660,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="324" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>339</v>
       </c>
@@ -29749,7 +29746,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="325" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>460</v>
       </c>
@@ -29912,7 +29909,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="327" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>361</v>
       </c>
@@ -29998,7 +29995,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="328" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>361</v>
       </c>
@@ -30078,7 +30075,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="329" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>364</v>
       </c>
@@ -30155,7 +30152,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="330" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>364</v>
       </c>
@@ -30241,7 +30238,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="331" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>367</v>
       </c>
@@ -30327,7 +30324,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="332" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>367</v>
       </c>
@@ -30413,7 +30410,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="333" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>367</v>
       </c>
@@ -30499,7 +30496,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="334" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>369</v>
       </c>
@@ -30576,7 +30573,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="335" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>369</v>
       </c>
@@ -30662,7 +30659,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="336" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>376</v>
       </c>
@@ -30748,7 +30745,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="337" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>376</v>
       </c>
@@ -30834,7 +30831,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="338" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>376</v>
       </c>
@@ -30920,7 +30917,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="339" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>377</v>
       </c>
@@ -31006,7 +31003,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="340" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>377</v>
       </c>
@@ -31092,7 +31089,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="341" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>379</v>
       </c>
@@ -31178,7 +31175,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="342" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>379</v>
       </c>
@@ -31264,7 +31261,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="343" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>379</v>
       </c>
@@ -31608,7 +31605,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="347" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>423</v>
       </c>
@@ -31694,7 +31691,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="348" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>423</v>
       </c>
@@ -31780,7 +31777,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="349" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>423</v>
       </c>
@@ -31866,7 +31863,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="350" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>424</v>
       </c>
@@ -31952,7 +31949,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="351" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>424</v>
       </c>
@@ -32038,7 +32035,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="352" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>424</v>
       </c>
@@ -32124,7 +32121,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="353" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>460</v>
       </c>
@@ -32382,7 +32379,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="356" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>466</v>
       </c>
@@ -32468,7 +32465,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="357" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>466</v>
       </c>
@@ -32554,7 +32551,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="358" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>466</v>
       </c>
@@ -32723,7 +32720,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="360" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>476</v>
       </c>
@@ -32892,7 +32889,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="362" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>14.1</v>
       </c>
@@ -32978,7 +32975,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="363" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>14.1</v>
       </c>
@@ -33064,7 +33061,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="364" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>14.1</v>
       </c>
@@ -33150,7 +33147,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="365" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>14.2</v>
       </c>
@@ -33236,7 +33233,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="366" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>14.2</v>
       </c>
@@ -33322,7 +33319,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="367" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>14.2</v>
       </c>
@@ -33408,7 +33405,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="368" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>14.3</v>
       </c>
@@ -33494,7 +33491,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="369" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>14.3</v>
       </c>
@@ -33580,7 +33577,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="370" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>14.3</v>
       </c>
@@ -33666,7 +33663,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="371" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>14.4</v>
       </c>
@@ -33752,7 +33749,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="372" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>14.4</v>
       </c>
@@ -33838,7 +33835,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="373" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>14.4</v>
       </c>
@@ -34440,7 +34437,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="380" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>228</v>
       </c>
@@ -34526,7 +34523,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="381" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>476</v>
       </c>
@@ -34612,7 +34609,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="382" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>460</v>
       </c>
@@ -34698,7 +34695,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="383" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>148</v>
       </c>
@@ -34784,7 +34781,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="384" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>339</v>
       </c>
@@ -34870,7 +34867,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="385" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>325</v>
       </c>
@@ -34956,7 +34953,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="386" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>323</v>
       </c>
@@ -35042,7 +35039,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="387" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>276</v>
       </c>
@@ -35128,7 +35125,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="388" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A388">
         <v>14</v>
       </c>
@@ -35214,7 +35211,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="389" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A389">
         <v>379</v>
       </c>
@@ -35300,7 +35297,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="390" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A390">
         <v>274</v>
       </c>
@@ -35386,7 +35383,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="391" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>14.1</v>
       </c>
@@ -35472,7 +35469,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="392" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>14.2</v>
       </c>
@@ -35558,7 +35555,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="393" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A393">
         <v>14.3</v>
       </c>
@@ -35644,7 +35641,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="394" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A394">
         <v>14.4</v>
       </c>
@@ -35730,7 +35727,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="395" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>423</v>
       </c>
@@ -35816,7 +35813,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="396" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>97</v>
       </c>
@@ -35896,7 +35893,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="397" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A397">
         <v>98</v>
       </c>
@@ -35982,7 +35979,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="398" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>194</v>
       </c>
@@ -36068,7 +36065,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="399" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>193</v>
       </c>
@@ -36154,7 +36151,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="400" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A400">
         <v>466</v>
       </c>
@@ -36240,7 +36237,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="401" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A401">
         <v>245</v>
       </c>
@@ -36326,7 +36323,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="402" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A402">
         <v>205</v>
       </c>
@@ -36412,7 +36409,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="403" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A403">
         <v>204</v>
       </c>
@@ -36498,7 +36495,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="404" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A404">
         <v>377</v>
       </c>
@@ -36584,7 +36581,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="405" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A405">
         <v>367</v>
       </c>
@@ -36670,7 +36667,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="406" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A406">
         <v>364</v>
       </c>
@@ -36756,7 +36753,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="407" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A407">
         <v>376</v>
       </c>
@@ -36842,7 +36839,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="408" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A408">
         <v>228</v>
       </c>
@@ -36928,7 +36925,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="409" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A409">
         <v>203</v>
       </c>
@@ -37014,7 +37011,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="410" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A410">
         <v>207</v>
       </c>
@@ -37100,7 +37097,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="411" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A411">
         <v>361</v>
       </c>
@@ -37186,7 +37183,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="412" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A412">
         <v>244</v>
       </c>
@@ -37272,7 +37269,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="413" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A413">
         <v>369</v>
       </c>
@@ -37358,7 +37355,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="414" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A414">
         <v>331</v>
       </c>
@@ -38031,7 +38028,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="422" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A422">
         <v>424</v>
       </c>
@@ -38117,7 +38114,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="423" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A423">
         <v>277</v>
       </c>
@@ -38521,14 +38518,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC427" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="22">
-      <filters>
-        <filter val="Educación_para_toda_la_vida"/>
-        <filter val="Transformación_Organizacional"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AC427" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>